<commit_message>
updated control design block diagram to account all phenomena which we know of right now
includes saturation of the PWM and position values, limit switches, sheave sliding due to belt tension, and change of the throttle position
</commit_message>
<xml_diff>
--- a/eCVT_step_response/ecvt_step_response2.xlsx
+++ b/eCVT_step_response/ecvt_step_response2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\Programs\bruin-racing-baja\eCVT_step_response\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69BB928-CC4A-4D59-83A1-018BE4CAA758}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEDEE7F-8DBE-4F12-B39B-FF6EDC742591}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C5EA4D49-530C-4EB9-8A06-62B87964F5CD}"/>
   </bookViews>
@@ -14386,16 +14386,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14422,16 +14422,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14759,7 +14759,7 @@
   <dimension ref="A1:I837"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>